<commit_message>
feat: improve Excel import template for guru with validation notes and examples
</commit_message>
<xml_diff>
--- a/public/template_excel/data-guru.xlsx
+++ b/public/template_excel/data-guru.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ujikom~Absensi\Absensi\public\template_excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Projects\Laravel\Unmaintained\PresensiSiswa\public\template_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C17A7B28-9347-4036-A2EC-CE5AA61E4293}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{052196C5-548A-4791-B7DF-DE86D8F0FE68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2505" yWindow="2505" windowWidth="15375" windowHeight="7995" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="KETENTUAN PENGISIAN DATA" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,25 +26,332 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>nip</t>
-  </si>
-  <si>
-    <t>nama_lengkap</t>
-  </si>
-  <si>
-    <t>jenis_kelamin</t>
-  </si>
-  <si>
-    <t>no_telepon</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
+  <si>
+    <t xml:space="preserve">    Data Guru
+</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>NIP</t>
+  </si>
+  <si>
+    <t>Nama Lengkap</t>
+  </si>
+  <si>
+    <t>Jenis Kelamin</t>
+  </si>
+  <si>
+    <t>Nomor Telepon</t>
+  </si>
+  <si>
+    <t>Ketentuan:</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. Kolom NIP </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>wajib diisi</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, dan harus terdiri dari</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> tepat 18 digit angka</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. Tidak boleh lebih, kurang, atau mengandung huruf/simbol.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">3. Kolom </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Jenis Kelamin</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> hanya boleh diisi salah satu dari: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Laki-laki atau Perempuan</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. Harap perhatikan kapitalisasi &amp; spasi.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">4. Kolom </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Nomor Telepon</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> wajib diisi, hanya boleh berisi angka, dan maksimal 13 digit. Tidak boleh ada spasi atau tanda baca.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">5. Data </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>NIP dan Nomor Telepon</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> tidak boleh ada yang sama </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>di dalam file ini</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, maupun yang </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>sudah pernah terdaftar sebelumnya</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">6. Pastikan </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>tidak ada kolom yang kosong</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. Data yang tidak lengkap akan diabaikan.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Contoh pengisian yang benar: </t>
+  </si>
+  <si>
+    <t>Rizky Maulana</t>
+  </si>
+  <si>
+    <t>Laki-laki</t>
+  </si>
+  <si>
+    <t>0817456321982</t>
+  </si>
+  <si>
+    <t>Ayu Kartikasari</t>
+  </si>
+  <si>
+    <t>Perempuan</t>
+  </si>
+  <si>
+    <t>0821345678912</t>
+  </si>
+  <si>
+    <t>Putri Maharani</t>
+  </si>
+  <si>
+    <t>0819023847165</t>
+  </si>
+  <si>
+    <t>100283746592837000</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">2. Kolom </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Nama Lengkap wajib diisi</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, dan tidak boleh lebih dari </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>100 karakter</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (termasuk spasi &amp; simbol).</t>
+    </r>
+  </si>
+  <si>
+    <t>7. Gunakan format Teks pada kolom NIP dan Nomor Telepon. Jika tidak, angka bisa berubah (misal: nol di depan hilang, atau jadi format ilmiah seperti 1.2E+17).</t>
+  </si>
+  <si>
+    <t>*Data di atas hanya contoh. Tidak mengacu pada data sebenarnya.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -55,6 +363,46 @@
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -64,7 +412,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -72,12 +420,133 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -91,6 +560,51 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -372,91 +886,136 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:N22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14" style="2" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="32" customWidth="1"/>
+    <col min="4" max="4" width="23.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="25.28515625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="59.42578125" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:14" ht="15.75">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+    </row>
+    <row r="2" spans="1:14" ht="15.75">
+      <c r="A2" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B2" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="C2" s="33" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="3"/>
-      <c r="D2" s="5"/>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="D2" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
+    </row>
+    <row r="3" spans="1:14">
       <c r="A3" s="3"/>
       <c r="D3" s="5"/>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
+    </row>
+    <row r="4" spans="1:14">
       <c r="A4" s="4"/>
       <c r="D4" s="5"/>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
+      <c r="M4" s="8"/>
+      <c r="N4" s="8"/>
+    </row>
+    <row r="5" spans="1:14">
       <c r="A5" s="4"/>
       <c r="D5" s="5"/>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="8"/>
+      <c r="N5" s="8"/>
+    </row>
+    <row r="6" spans="1:14">
       <c r="A6" s="4"/>
       <c r="D6" s="5"/>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="8"/>
+      <c r="N6" s="8"/>
+    </row>
+    <row r="7" spans="1:14">
       <c r="A7" s="4"/>
       <c r="D7" s="5"/>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="8"/>
+      <c r="M7" s="8"/>
+      <c r="N7" s="8"/>
+    </row>
+    <row r="8" spans="1:14">
       <c r="A8" s="4"/>
       <c r="D8" s="5"/>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="8"/>
+      <c r="M8" s="8"/>
+      <c r="N8" s="8"/>
+    </row>
+    <row r="9" spans="1:14">
       <c r="A9" s="4"/>
       <c r="D9" s="5"/>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:14">
       <c r="A10" s="4"/>
       <c r="D10" s="5"/>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:14">
       <c r="A11" s="4"/>
       <c r="D11" s="5"/>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:14">
       <c r="A12" s="4"/>
       <c r="D12" s="5"/>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:14">
       <c r="A13" s="4"/>
       <c r="D13" s="5"/>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:14">
       <c r="A14" s="4"/>
       <c r="D14" s="5"/>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:14">
       <c r="A15" s="4"/>
       <c r="D15" s="5"/>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:14">
       <c r="A16" s="4"/>
       <c r="D16" s="5"/>
     </row>
@@ -485,6 +1044,288 @@
       <c r="D22" s="6"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9054F69-B387-40EF-A7CA-7D8884537E72}">
+  <dimension ref="A1:M17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="19.5703125" customWidth="1"/>
+    <col min="3" max="3" width="23.85546875" customWidth="1"/>
+    <col min="4" max="4" width="25" customWidth="1"/>
+    <col min="5" max="5" width="53.5703125" customWidth="1"/>
+    <col min="6" max="6" width="45" customWidth="1"/>
+    <col min="13" max="13" width="35.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="18.75">
+      <c r="A1" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
+      <c r="M1" s="25"/>
+    </row>
+    <row r="2" spans="1:13" ht="18.75">
+      <c r="A2" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
+      <c r="K2" s="24"/>
+      <c r="L2" s="24"/>
+      <c r="M2" s="24"/>
+    </row>
+    <row r="3" spans="1:13" ht="18.75">
+      <c r="A3" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="24"/>
+      <c r="J3" s="24"/>
+      <c r="K3" s="24"/>
+      <c r="L3" s="24"/>
+      <c r="M3" s="24"/>
+    </row>
+    <row r="4" spans="1:13" ht="18.75">
+      <c r="A4" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="24"/>
+      <c r="K4" s="24"/>
+      <c r="L4" s="24"/>
+      <c r="M4" s="24"/>
+    </row>
+    <row r="5" spans="1:13" ht="18.75">
+      <c r="A5" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="24"/>
+      <c r="I5" s="24"/>
+      <c r="J5" s="24"/>
+      <c r="K5" s="24"/>
+      <c r="L5" s="24"/>
+      <c r="M5" s="24"/>
+    </row>
+    <row r="6" spans="1:13" s="10" customFormat="1" ht="18.75">
+      <c r="A6" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="24"/>
+      <c r="J6" s="24"/>
+      <c r="K6" s="24"/>
+      <c r="L6" s="24"/>
+      <c r="M6" s="24"/>
+    </row>
+    <row r="7" spans="1:13" ht="18.75">
+      <c r="A7" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="27"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="29"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="26"/>
+      <c r="I7" s="26"/>
+      <c r="J7" s="26"/>
+      <c r="K7" s="26"/>
+      <c r="L7" s="26"/>
+      <c r="M7" s="26"/>
+    </row>
+    <row r="8" spans="1:13" ht="18.75">
+      <c r="A8" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="30"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="31"/>
+    </row>
+    <row r="9" spans="1:13" ht="18.75">
+      <c r="D9" s="28"/>
+      <c r="E9" s="28"/>
+      <c r="F9" s="28"/>
+      <c r="G9" s="28"/>
+      <c r="H9" s="28"/>
+      <c r="I9" s="28"/>
+      <c r="J9" s="28"/>
+      <c r="K9" s="28"/>
+      <c r="L9" s="28"/>
+      <c r="M9" s="28"/>
+    </row>
+    <row r="10" spans="1:13" ht="18.75">
+      <c r="A10" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="35"/>
+      <c r="C10" s="35"/>
+      <c r="D10" s="35"/>
+      <c r="E10" s="35"/>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11" s="36"/>
+      <c r="B11" s="36"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="36"/>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="18"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E13" s="20" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="A14" s="21">
+        <v>1</v>
+      </c>
+      <c r="B14" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" s="22" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="A15" s="21">
+        <v>2</v>
+      </c>
+      <c r="B15" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" s="22" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="A16" s="21">
+        <v>3</v>
+      </c>
+      <c r="B16" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" s="22" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+    </row>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="A5:F5"/>
+    <mergeCell ref="A4:F4"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A8:F8"/>
+    <mergeCell ref="A12:E12"/>
+    <mergeCell ref="A7:F7"/>
+    <mergeCell ref="A6:F6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+</worksheet>
 </file>
</xml_diff>